<commit_message>
add fuzzy pid but not work
</commit_message>
<xml_diff>
--- a/hotter/协议.xlsx
+++ b/hotter/协议.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\Hardware\hotter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55BB9E4-7B12-4746-8566-08D25B876A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44373BE7-50C8-405C-A578-0168DEBBD594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="数据协议" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="主控板与设备协议" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>4-20ma</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,6 +84,306 @@
   </si>
   <si>
     <t>电阻1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变量名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mqtt_payload_u.status[DEV_STATUS_INDEX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位宽（bit）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地暖机故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>压力故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>di故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31-28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19-8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>故障位定义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应位为1代表有故障</t>
+  </si>
+  <si>
+    <t>对应位为1代表有故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取值范围0-15；
+0代表无故障；
+1-15代表15种故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制板与云服务器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MQTT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传本地设备状态，接收云端指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTTP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制板OTA升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>具体格式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>设备---&gt;云：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">发布1个主题，暂定为MPUB/devid,devid为控制板唯一标识号，控制板通过该主题实时发送本地设备状态；
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>云---&gt;设备：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>设备定订阅1个主题，暂定为MSUB/devid</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>故障结构（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>运行状态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>设备---&gt;云：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       升级机制：
+              1、控制板主动get云端固件版本号，如果版本不一致，进入升级模式；
+              2、控制板主动get请求，云服务先返回 ota固件的总长度；
+              3、控制板每get一次后，云端每次返回1kbyte+2个字节（crc)
+              4、crc校验错误，控制板会发送post请求，返回“data crc error”;
+              5、控制板继续get请求，云端根据有无返回值判断发送下一帧数据，还是重发上一帧数据</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上传云端数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：{
+    "设备ID": ”12111111111111111111111178787897“,
+    "运行数据": {
+        "出水温度": 45,
+        "回水温度": 26,
+        "泵前压力": 0.5,
+        "泵后压力": 0.5,
+        "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>运行状态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">": 4
+    },
+    "设备参数": {
+        "版本号": V3.0.1,
+        "设置出水温度": 45,
+        "设置室内温度": 23,
+        "数据上传周期": 10
+    }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>服务端下发数据：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{
+   "设备ID": "12111111111111111111111178787897",
+   "设备控制": {
+               "升级": 1,
+               "重启": 1,
+               "机组开关机": 0,
+               "设置出水温度": 45,
+               "设置室内温度": 23,
+               "数据上传周期": 20
+        }
+}</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -88,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +401,31 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -124,8 +452,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -141,6 +484,121 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>78209</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>160693</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB95CB95-A98F-E0E5-5DA9-BA578306D483}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1682750"/>
+          <a:ext cx="9323809" cy="9857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCEB961-FADA-4E0A-AA3D-6D7617AC4032}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7219950" y="8750300"/>
+          <a:ext cx="927100" cy="2876550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="50800">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -523,4 +981,202 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C17B224-1F09-4905-ACA2-599DDA3A966A}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="72.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1"/>
+    <col min="5" max="5" width="18.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="364" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="126" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="E27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="E28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665AB449-856B-4BEF-8A0C-9B5A628FA79A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BE9F0A-F1BA-47B4-ACC1-0F26B26FF142}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>